<commit_message>
revised bom for larger programming pin
</commit_message>
<xml_diff>
--- a/BOM - Remote Monitoring Hardware.xlsx
+++ b/BOM - Remote Monitoring Hardware.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82d73bfb70c174d8/Documents/New folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Desktop\work\Remote Monitoring Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="9D6399416B2645C07C67A63B7EF868BE9204DDB8" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{4F4DCC25-DB8C-491D-9948-F60B0AF6592D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +92,6 @@
     <t>J7</t>
   </si>
   <si>
-    <t>53047-06</t>
-  </si>
-  <si>
     <t>LED_1206</t>
   </si>
   <si>
@@ -213,9 +209,6 @@
     <t>MAX31855TASA+</t>
   </si>
   <si>
-    <t>CONN HEADER .050" 6POS PCB GOLD</t>
-  </si>
-  <si>
     <t>L1, L2</t>
   </si>
   <si>
@@ -429,16 +422,22 @@
     <t>LP-21PMBT</t>
   </si>
   <si>
-    <t>S9008E-06-ND</t>
-  </si>
-  <si>
-    <t>LPPB061NFFN-RC</t>
-  </si>
-  <si>
     <t>609-3271-ND</t>
   </si>
   <si>
     <t>68001-104HLF</t>
+  </si>
+  <si>
+    <t>609-3272-ND</t>
+  </si>
+  <si>
+    <t>68001-106HLF</t>
+  </si>
+  <si>
+    <t>CONN HEADER 6POS .100 STR 30AU</t>
+  </si>
+  <si>
+    <t>MA06-1</t>
   </si>
 </sst>
 </file>
@@ -572,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -639,6 +638,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -987,43 +987,43 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="I1" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>133</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G2" s="12">
         <v>1</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>4</v>
@@ -1048,13 +1048,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="13">
         <v>2</v>
@@ -1067,7 +1067,7 @@
         <v>0.38</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1081,13 +1081,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="G4" s="13">
         <v>1</v>
@@ -1100,12 +1100,12 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>8</v>
@@ -1114,13 +1114,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="13">
         <v>2</v>
@@ -1133,27 +1133,27 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="G6" s="13">
         <v>3</v>
@@ -1166,7 +1166,7 @@
         <v>1.1099999999999999</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1180,13 +1180,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="G7" s="13">
         <v>1</v>
@@ -1199,27 +1199,27 @@
         <v>0.4</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="E8" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="F8" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="G8" s="13">
         <v>1</v>
@@ -1234,16 +1234,16 @@
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G9" s="11">
         <v>1</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>11</v>
@@ -1267,13 +1267,13 @@
         <v>12</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="G10" s="13">
         <v>2</v>
@@ -1286,27 +1286,27 @@
         <v>0.7</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="F11" s="21" t="s">
         <v>99</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>101</v>
       </c>
       <c r="G11" s="22">
         <v>1</v>
@@ -1319,7 +1319,7 @@
         <v>3.6</v>
       </c>
       <c r="K11" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>14</v>
@@ -1346,7 +1346,7 @@
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
       <c r="F13" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="13">
         <v>2</v>
@@ -1359,23 +1359,23 @@
         <v>2</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>103</v>
+        <v>83</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G14" s="22">
         <v>1</v>
@@ -1388,7 +1388,7 @@
         <v>23.49</v>
       </c>
       <c r="K14" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1402,13 +1402,13 @@
         <v>17</v>
       </c>
       <c r="D15" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G15" s="13">
         <v>1</v>
@@ -1421,7 +1421,7 @@
         <v>7</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1437,18 +1437,18 @@
     </row>
     <row r="17" spans="1:11" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G17" s="22">
         <v>5</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
@@ -1483,25 +1483,25 @@
         <v>1.6500000000000001</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G19" s="13">
         <v>1</v>
@@ -1524,10 +1524,10 @@
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G20" s="7">
         <v>1</v>
@@ -1540,7 +1540,7 @@
         <v>0.41</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1548,11 +1548,11 @@
         <v>21</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="C21" s="12" t="s">
-        <v>22</v>
+      <c r="C21" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>134</v>
@@ -1564,32 +1564,32 @@
         <v>1</v>
       </c>
       <c r="H21" s="13">
-        <v>1.57</v>
+        <v>0.46</v>
       </c>
       <c r="I21" s="13">
         <f t="shared" si="1"/>
-        <v>1.57</v>
+        <v>0.46</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>66</v>
-      </c>
       <c r="F22" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="13">
         <v>2</v>
@@ -1602,27 +1602,27 @@
         <v>0.54</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G23" s="13">
         <v>3</v>
@@ -1635,27 +1635,27 @@
         <v>2.16</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>26</v>
-      </c>
       <c r="C24" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="G24" s="13">
         <v>1</v>
@@ -1668,27 +1668,27 @@
         <v>0.59</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D25" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>113</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="G25" s="13">
         <v>1</v>
@@ -1701,27 +1701,27 @@
         <v>0.59</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="D26" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G26" s="13">
         <v>1</v>
@@ -1734,7 +1734,7 @@
         <v>0.15</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1783,22 +1783,22 @@
     </row>
     <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>29</v>
-      </c>
       <c r="E31" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G31" s="13">
         <v>2</v>
@@ -1811,27 +1811,27 @@
         <v>0.3</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>29</v>
-      </c>
       <c r="E32" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G32" s="13">
         <v>4</v>
@@ -1844,7 +1844,7 @@
         <v>0.6</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1860,20 +1860,20 @@
     </row>
     <row r="34" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G34" s="13">
         <v>1</v>
@@ -1886,7 +1886,7 @@
         <v>1.19</v>
       </c>
       <c r="K34" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1928,19 +1928,19 @@
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="13">
         <f>SUM(I2:I35)</f>
-        <v>69.819999999999993</v>
+        <v>68.709999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F40" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>